<commit_message>
Change the test case by Gilana and Waseem
</commit_message>
<xml_diff>
--- a/DOCS/Test Cases/TC01-Create Crisis.xlsx
+++ b/DOCS/Test Cases/TC01-Create Crisis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Intput Type</t>
   </si>
@@ -84,21 +84,12 @@
     <t>Create a crisis with 3 letters</t>
   </si>
   <si>
-    <t>O1:Ore</t>
-  </si>
-  <si>
     <t>Explanation:</t>
   </si>
   <si>
     <t>Testcase ID: First two numbers is the use case number, second two numbers are remaining test case number. Input Explanation: O1 means option 1 will be selected for this case. Ore is the example to use in test case.</t>
   </si>
   <si>
-    <t>Earthquake</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
     <t>O1:Earthquake</t>
   </si>
   <si>
@@ -121,6 +112,66 @@
   </si>
   <si>
     <t>Error Message</t>
+  </si>
+  <si>
+    <t>Crisis Location Name</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Letters</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Letters and Numbers</t>
+  </si>
+  <si>
+    <t>Create a crisis with out location name</t>
+  </si>
+  <si>
+    <t>O1:&lt;space&gt;</t>
+  </si>
+  <si>
+    <t>O1:Abc</t>
+  </si>
+  <si>
+    <t>Create a crisis with only numbers in location name</t>
+  </si>
+  <si>
+    <t>O3:3278648</t>
+  </si>
+  <si>
+    <t>TC01.03</t>
+  </si>
+  <si>
+    <t>TC01.04</t>
+  </si>
+  <si>
+    <t>O3:Abc 23</t>
+  </si>
+  <si>
+    <t>O3:Abcdfg</t>
+  </si>
+  <si>
+    <t>Selected</t>
+  </si>
+  <si>
+    <t>TC01.05</t>
+  </si>
+  <si>
+    <t>Create crisis without selecting Crisis Type</t>
+  </si>
+  <si>
+    <t>O2:Abc</t>
+  </si>
+  <si>
+    <t>&lt;Not selected&gt;</t>
+  </si>
+  <si>
+    <t>O2:&lt;not selected&gt;</t>
   </si>
 </sst>
 </file>
@@ -598,14 +649,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="9" width="17.5703125" customWidth="1"/>
+    <col min="2" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="9" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
@@ -637,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -657,11 +712,9 @@
         <v>11</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9">
@@ -669,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -681,12 +734,22 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -891,26 +954,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="10" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -949,7 +1019,9 @@
       <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -957,38 +1029,104 @@
       <c r="J3" s="6"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="30.75" thickTop="1">
+    <row r="4" spans="1:11" ht="33.75" customHeight="1" thickTop="1">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21" customHeight="1">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s">
+      <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="30">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
+    </row>
+    <row r="6" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1007,7 +1145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>